<commit_message>
background modified and coordinates
</commit_message>
<xml_diff>
--- a/assets/CONTROL 678_2024-1 - EVALUACIÓN - STP - CAMIÓN ALJIBE - LYLG-45.xlsx
+++ b/assets/CONTROL 678_2024-1 - EVALUACIÓN - STP - CAMIÓN ALJIBE - LYLG-45.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://prominet1-my.sharepoint.com/personal/vsepulveda_prominet_cl/Documents/PROMINET - OPERACIONES/9. OT 2024/678_2024-1 - EVALUACIÓN - STP - CAMIÓN ALJIBE - LYLG-45/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ADL\Desafios\excelToPptApp\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="11_69B8722D8AEDF7C04F9D376D0A5467F33BF6DA54" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CF1458A-D3B9-46D9-96BA-8F2CE8BF463B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C915B2-8BA2-413A-9357-445E042DE103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -471,7 +471,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="###0;###0"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1380,37 +1380,16 @@
     <xf numFmtId="0" fontId="11" fillId="9" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1422,8 +1401,29 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1435,6 +1435,34 @@
   </cellStyles>
   <dxfs count="123">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1446,39 +1474,21 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1509,16 +1519,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5200,13 +5200,13 @@
   <dimension ref="B2:V53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="8" topLeftCell="G42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="8" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G44" sqref="G44:H50"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.109375" customWidth="1"/>
     <col min="2" max="2" width="2.44140625" customWidth="1"/>
@@ -5232,7 +5232,7 @@
     <col min="22" max="22" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:22">
+    <row r="2" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -5242,7 +5242,7 @@
       <c r="H2" s="97"/>
       <c r="I2" s="97"/>
     </row>
-    <row r="3" spans="2:22" ht="14.4" customHeight="1">
+    <row r="3" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3"/>
       <c r="C3" s="38"/>
       <c r="D3" s="38"/>
@@ -5259,7 +5259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:22" ht="14.4" customHeight="1">
+    <row r="4" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3"/>
       <c r="C4" s="38"/>
       <c r="D4" s="38"/>
@@ -5274,7 +5274,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="2:22" ht="14.4" customHeight="1">
+    <row r="5" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
       <c r="C5" s="38"/>
       <c r="D5" s="38"/>
@@ -5289,7 +5289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:22" ht="15" thickBot="1">
+    <row r="6" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="3"/>
       <c r="C6" s="38"/>
       <c r="D6" s="38"/>
@@ -5312,14 +5312,14 @@
       <c r="U6" s="31"/>
       <c r="V6" s="3"/>
     </row>
-    <row r="7" spans="2:22" ht="26.4" thickBot="1">
+    <row r="7" spans="2:22" ht="26.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="3"/>
       <c r="C7" s="87" t="s">
         <v>83</v>
       </c>
       <c r="D7" s="86">
         <f ca="1">TODAY()</f>
-        <v>45495</v>
+        <v>45496</v>
       </c>
       <c r="E7" s="42"/>
       <c r="F7" s="92"/>
@@ -5345,11 +5345,11 @@
       </c>
       <c r="U7" s="90">
         <f ca="1">TODAY()</f>
-        <v>45495</v>
+        <v>45496</v>
       </c>
       <c r="V7" s="3"/>
     </row>
-    <row r="8" spans="2:22" ht="15.6">
+    <row r="8" spans="2:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
       <c r="C8" s="51" t="s">
         <v>84</v>
@@ -5408,7 +5408,7 @@
       </c>
       <c r="V8" s="3"/>
     </row>
-    <row r="9" spans="2:22">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
       <c r="C9" s="85" t="s">
         <v>85</v>
@@ -5442,7 +5442,7 @@
       <c r="U9" s="84"/>
       <c r="V9" s="3"/>
     </row>
-    <row r="10" spans="2:22">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>
       <c r="C10" s="85" t="s">
         <v>85</v>
@@ -5476,7 +5476,7 @@
       <c r="U10" s="84"/>
       <c r="V10" s="3"/>
     </row>
-    <row r="11" spans="2:22">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
       <c r="C11" s="85" t="s">
         <v>85</v>
@@ -5510,7 +5510,7 @@
       <c r="U11" s="84"/>
       <c r="V11" s="3"/>
     </row>
-    <row r="12" spans="2:22">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
       <c r="C12" s="85" t="s">
         <v>85</v>
@@ -5544,7 +5544,7 @@
       <c r="U12" s="84"/>
       <c r="V12" s="3"/>
     </row>
-    <row r="13" spans="2:22">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
       <c r="C13" s="85" t="s">
         <v>85</v>
@@ -5578,7 +5578,7 @@
       <c r="U13" s="84"/>
       <c r="V13" s="3"/>
     </row>
-    <row r="14" spans="2:22">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
       <c r="C14" s="85" t="s">
         <v>85</v>
@@ -5612,7 +5612,7 @@
       <c r="U14" s="84"/>
       <c r="V14" s="3"/>
     </row>
-    <row r="15" spans="2:22">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
       <c r="C15" s="85" t="s">
         <v>85</v>
@@ -5646,7 +5646,7 @@
       <c r="U15" s="84"/>
       <c r="V15" s="3"/>
     </row>
-    <row r="16" spans="2:22">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
       <c r="C16" s="85" t="s">
         <v>85</v>
@@ -5680,7 +5680,7 @@
       <c r="U16" s="84"/>
       <c r="V16" s="3"/>
     </row>
-    <row r="17" spans="2:22">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
       <c r="C17" s="85" t="s">
         <v>85</v>
@@ -5714,7 +5714,7 @@
       <c r="U17" s="84"/>
       <c r="V17" s="3"/>
     </row>
-    <row r="18" spans="2:22">
+    <row r="18" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
       <c r="C18" s="85" t="s">
         <v>85</v>
@@ -5748,7 +5748,7 @@
       <c r="U18" s="84"/>
       <c r="V18" s="3"/>
     </row>
-    <row r="19" spans="2:22">
+    <row r="19" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
       <c r="C19" s="85" t="s">
         <v>85</v>
@@ -5782,7 +5782,7 @@
       <c r="U19" s="84"/>
       <c r="V19" s="3"/>
     </row>
-    <row r="20" spans="2:22">
+    <row r="20" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B20" s="3"/>
       <c r="C20" s="85" t="s">
         <v>85</v>
@@ -5816,7 +5816,7 @@
       <c r="U20" s="84"/>
       <c r="V20" s="3"/>
     </row>
-    <row r="21" spans="2:22">
+    <row r="21" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B21" s="3"/>
       <c r="C21" s="85" t="s">
         <v>85</v>
@@ -5850,7 +5850,7 @@
       <c r="U21" s="84"/>
       <c r="V21" s="3"/>
     </row>
-    <row r="22" spans="2:22">
+    <row r="22" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B22" s="3"/>
       <c r="C22" s="85" t="s">
         <v>85</v>
@@ -5884,7 +5884,7 @@
       <c r="U22" s="84"/>
       <c r="V22" s="3"/>
     </row>
-    <row r="23" spans="2:22">
+    <row r="23" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B23" s="3"/>
       <c r="C23" s="85" t="s">
         <v>85</v>
@@ -5918,7 +5918,7 @@
       <c r="U23" s="84"/>
       <c r="V23" s="3"/>
     </row>
-    <row r="24" spans="2:22">
+    <row r="24" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B24" s="3"/>
       <c r="C24" s="85" t="s">
         <v>85</v>
@@ -5952,7 +5952,7 @@
       <c r="U24" s="84"/>
       <c r="V24" s="3"/>
     </row>
-    <row r="25" spans="2:22">
+    <row r="25" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B25" s="3"/>
       <c r="C25" s="85" t="s">
         <v>85</v>
@@ -5986,7 +5986,7 @@
       <c r="U25" s="84"/>
       <c r="V25" s="3"/>
     </row>
-    <row r="26" spans="2:22">
+    <row r="26" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B26" s="3"/>
       <c r="C26" s="85" t="s">
         <v>85</v>
@@ -6020,7 +6020,7 @@
       <c r="U26" s="84"/>
       <c r="V26" s="3"/>
     </row>
-    <row r="27" spans="2:22">
+    <row r="27" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B27" s="3"/>
       <c r="C27" s="85" t="s">
         <v>85</v>
@@ -6054,7 +6054,7 @@
       <c r="U27" s="84"/>
       <c r="V27" s="3"/>
     </row>
-    <row r="28" spans="2:22">
+    <row r="28" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B28" s="3"/>
       <c r="C28" s="85" t="s">
         <v>85</v>
@@ -6088,7 +6088,7 @@
       <c r="U28" s="84"/>
       <c r="V28" s="3"/>
     </row>
-    <row r="29" spans="2:22">
+    <row r="29" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B29" s="3"/>
       <c r="C29" s="85" t="s">
         <v>85</v>
@@ -6122,7 +6122,7 @@
       <c r="U29" s="84"/>
       <c r="V29" s="3"/>
     </row>
-    <row r="30" spans="2:22">
+    <row r="30" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B30" s="3"/>
       <c r="C30" s="85" t="s">
         <v>85</v>
@@ -6156,7 +6156,7 @@
       <c r="U30" s="84"/>
       <c r="V30" s="3"/>
     </row>
-    <row r="31" spans="2:22">
+    <row r="31" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B31" s="3"/>
       <c r="C31" s="85" t="s">
         <v>85</v>
@@ -6190,7 +6190,7 @@
       <c r="U31" s="84"/>
       <c r="V31" s="3"/>
     </row>
-    <row r="32" spans="2:22">
+    <row r="32" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B32" s="3"/>
       <c r="C32" s="85" t="s">
         <v>85</v>
@@ -6224,7 +6224,7 @@
       <c r="U32" s="84"/>
       <c r="V32" s="3"/>
     </row>
-    <row r="33" spans="2:22">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B33" s="3"/>
       <c r="C33" s="85" t="s">
         <v>85</v>
@@ -6258,7 +6258,7 @@
       <c r="U33" s="84"/>
       <c r="V33" s="3"/>
     </row>
-    <row r="34" spans="2:22">
+    <row r="34" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B34" s="3"/>
       <c r="C34" s="85" t="s">
         <v>85</v>
@@ -6292,7 +6292,7 @@
       <c r="U34" s="84"/>
       <c r="V34" s="3"/>
     </row>
-    <row r="35" spans="2:22">
+    <row r="35" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B35" s="3"/>
       <c r="C35" s="85" t="s">
         <v>85</v>
@@ -6326,7 +6326,7 @@
       <c r="U35" s="84"/>
       <c r="V35" s="3"/>
     </row>
-    <row r="36" spans="2:22">
+    <row r="36" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B36" s="3"/>
       <c r="C36" s="85" t="s">
         <v>85</v>
@@ -6360,7 +6360,7 @@
       <c r="U36" s="84"/>
       <c r="V36" s="3"/>
     </row>
-    <row r="37" spans="2:22">
+    <row r="37" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B37" s="3"/>
       <c r="C37" s="85" t="s">
         <v>85</v>
@@ -6394,7 +6394,7 @@
       <c r="U37" s="84"/>
       <c r="V37" s="3"/>
     </row>
-    <row r="38" spans="2:22">
+    <row r="38" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B38" s="3"/>
       <c r="C38" s="85" t="s">
         <v>85</v>
@@ -6428,7 +6428,7 @@
       <c r="U38" s="84"/>
       <c r="V38" s="3"/>
     </row>
-    <row r="39" spans="2:22">
+    <row r="39" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B39" s="3"/>
       <c r="C39" s="85" t="s">
         <v>85</v>
@@ -6462,7 +6462,7 @@
       <c r="U39" s="84"/>
       <c r="V39" s="3"/>
     </row>
-    <row r="40" spans="2:22">
+    <row r="40" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B40" s="3"/>
       <c r="C40" s="85" t="s">
         <v>85</v>
@@ -6496,7 +6496,7 @@
       <c r="U40" s="84"/>
       <c r="V40" s="3"/>
     </row>
-    <row r="41" spans="2:22">
+    <row r="41" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B41" s="3"/>
       <c r="C41" s="85" t="s">
         <v>85</v>
@@ -6530,7 +6530,7 @@
       <c r="U41" s="84"/>
       <c r="V41" s="3"/>
     </row>
-    <row r="42" spans="2:22">
+    <row r="42" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B42" s="3"/>
       <c r="C42" s="85" t="s">
         <v>85</v>
@@ -6564,7 +6564,7 @@
       <c r="U42" s="84"/>
       <c r="V42" s="3"/>
     </row>
-    <row r="43" spans="2:22">
+    <row r="43" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B43" s="3"/>
       <c r="C43" s="85" t="s">
         <v>85</v>
@@ -6598,7 +6598,7 @@
       <c r="U43" s="84"/>
       <c r="V43" s="3"/>
     </row>
-    <row r="44" spans="2:22">
+    <row r="44" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B44" s="3"/>
       <c r="C44" s="85" t="s">
         <v>85</v>
@@ -6632,7 +6632,7 @@
       <c r="U44" s="84"/>
       <c r="V44" s="3"/>
     </row>
-    <row r="45" spans="2:22">
+    <row r="45" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B45" s="3"/>
       <c r="C45" s="85" t="s">
         <v>85</v>
@@ -6666,7 +6666,7 @@
       <c r="U45" s="84"/>
       <c r="V45" s="3"/>
     </row>
-    <row r="46" spans="2:22">
+    <row r="46" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B46" s="3"/>
       <c r="C46" s="85" t="s">
         <v>85</v>
@@ -6700,7 +6700,7 @@
       <c r="U46" s="84"/>
       <c r="V46" s="3"/>
     </row>
-    <row r="47" spans="2:22">
+    <row r="47" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B47" s="3"/>
       <c r="C47" s="85" t="s">
         <v>85</v>
@@ -6734,7 +6734,7 @@
       <c r="U47" s="84"/>
       <c r="V47" s="3"/>
     </row>
-    <row r="48" spans="2:22">
+    <row r="48" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B48" s="3"/>
       <c r="C48" s="85" t="s">
         <v>85</v>
@@ -6768,7 +6768,7 @@
       <c r="U48" s="84"/>
       <c r="V48" s="3"/>
     </row>
-    <row r="49" spans="2:22">
+    <row r="49" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B49" s="3"/>
       <c r="C49" s="85" t="s">
         <v>85</v>
@@ -6802,7 +6802,7 @@
       <c r="U49" s="84"/>
       <c r="V49" s="3"/>
     </row>
-    <row r="50" spans="2:22">
+    <row r="50" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B50" s="3"/>
       <c r="C50" s="85" t="s">
         <v>85</v>
@@ -6836,7 +6836,7 @@
       <c r="U50" s="84"/>
       <c r="V50" s="3"/>
     </row>
-    <row r="51" spans="2:22">
+    <row r="51" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B51" s="3"/>
       <c r="C51" s="85" t="s">
         <v>85</v>
@@ -6845,7 +6845,7 @@
         <v>62</v>
       </c>
       <c r="E51" s="84">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="F51" s="89" t="s">
         <v>60</v>
@@ -6870,7 +6870,7 @@
       <c r="U51" s="84"/>
       <c r="V51" s="3"/>
     </row>
-    <row r="52" spans="2:22">
+    <row r="52" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B52" s="3"/>
       <c r="C52" s="85" t="s">
         <v>85</v>
@@ -6879,7 +6879,7 @@
         <v>62</v>
       </c>
       <c r="E52" s="84">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F52" s="89" t="s">
         <v>61</v>
@@ -6904,7 +6904,7 @@
       <c r="U52" s="84"/>
       <c r="V52" s="3"/>
     </row>
-    <row r="53" spans="2:22">
+    <row r="53" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -7360,12 +7360,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G44:G50">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44:H50">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7383,7 +7383,7 @@
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
     <col min="2" max="2" width="13.88671875" customWidth="1"/>
@@ -7395,7 +7395,7 @@
     <col min="9" max="9" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="18">
+    <row r="2" spans="2:9" ht="18" x14ac:dyDescent="0.3">
       <c r="B2" s="45"/>
       <c r="C2" s="45"/>
       <c r="D2" s="101" t="s">
@@ -7407,7 +7407,7 @@
       <c r="H2" s="101"/>
       <c r="I2" s="101"/>
     </row>
-    <row r="3" spans="2:9" ht="18">
+    <row r="3" spans="2:9" ht="18" x14ac:dyDescent="0.3">
       <c r="B3" s="45"/>
       <c r="C3" s="45"/>
       <c r="D3" s="101"/>
@@ -7417,7 +7417,7 @@
       <c r="H3" s="101"/>
       <c r="I3" s="101"/>
     </row>
-    <row r="4" spans="2:9" ht="18">
+    <row r="4" spans="2:9" ht="18" x14ac:dyDescent="0.3">
       <c r="B4" s="45"/>
       <c r="C4" s="45"/>
       <c r="D4" s="101"/>
@@ -7427,7 +7427,7 @@
       <c r="H4" s="101"/>
       <c r="I4" s="101"/>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="61" t="s">
         <v>5</v>
       </c>
@@ -7451,7 +7451,7 @@
       </c>
       <c r="I5" s="102"/>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="100"/>
       <c r="C6" s="57"/>
       <c r="D6" s="58"/>
@@ -7461,7 +7461,7 @@
       <c r="H6" s="48"/>
       <c r="I6" s="48"/>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="100"/>
       <c r="C7" s="57"/>
       <c r="D7" s="58"/>
@@ -7471,7 +7471,7 @@
       <c r="H7" s="48"/>
       <c r="I7" s="48"/>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="100"/>
       <c r="C8" s="57"/>
       <c r="D8" s="58"/>
@@ -7481,7 +7481,7 @@
       <c r="H8" s="48"/>
       <c r="I8" s="48"/>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="100"/>
       <c r="C9" s="57"/>
       <c r="D9" s="58"/>
@@ -7491,7 +7491,7 @@
       <c r="H9" s="48"/>
       <c r="I9" s="48"/>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="100"/>
       <c r="C10" s="57"/>
       <c r="D10" s="58"/>
@@ -7501,7 +7501,7 @@
       <c r="H10" s="48"/>
       <c r="I10" s="48"/>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="100"/>
       <c r="C11" s="57"/>
       <c r="D11" s="58"/>
@@ -7511,7 +7511,7 @@
       <c r="H11" s="48"/>
       <c r="I11" s="48"/>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="100"/>
       <c r="C12" s="57"/>
       <c r="D12" s="58"/>
@@ -7521,7 +7521,7 @@
       <c r="H12" s="48"/>
       <c r="I12" s="48"/>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="100"/>
       <c r="C13" s="57"/>
       <c r="D13" s="58"/>
@@ -7531,7 +7531,7 @@
       <c r="H13" s="48"/>
       <c r="I13" s="48"/>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="100"/>
       <c r="C14" s="57"/>
       <c r="D14" s="58"/>
@@ -7541,7 +7541,7 @@
       <c r="H14" s="48"/>
       <c r="I14" s="48"/>
     </row>
-    <row r="15" spans="2:9">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="100"/>
       <c r="C15" s="57"/>
       <c r="D15" s="58"/>
@@ -7551,7 +7551,7 @@
       <c r="H15" s="48"/>
       <c r="I15" s="48"/>
     </row>
-    <row r="16" spans="2:9">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="100"/>
       <c r="C16" s="57"/>
       <c r="D16" s="60"/>
@@ -7561,7 +7561,7 @@
       <c r="H16" s="48"/>
       <c r="I16" s="48"/>
     </row>
-    <row r="17" spans="2:9">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="100"/>
       <c r="C17" s="57"/>
       <c r="D17" s="60"/>
@@ -7571,7 +7571,7 @@
       <c r="H17" s="48"/>
       <c r="I17" s="48"/>
     </row>
-    <row r="18" spans="2:9">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="100"/>
       <c r="C18" s="57"/>
       <c r="D18" s="60"/>
@@ -7581,7 +7581,7 @@
       <c r="H18" s="48"/>
       <c r="I18" s="48"/>
     </row>
-    <row r="19" spans="2:9">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="100"/>
       <c r="C19" s="57"/>
       <c r="D19" s="60"/>
@@ -7591,7 +7591,7 @@
       <c r="H19" s="48"/>
       <c r="I19" s="48"/>
     </row>
-    <row r="20" spans="2:9">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="100"/>
       <c r="C20" s="57"/>
       <c r="D20" s="60"/>
@@ -7601,7 +7601,7 @@
       <c r="H20" s="48"/>
       <c r="I20" s="48"/>
     </row>
-    <row r="21" spans="2:9">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="100"/>
       <c r="C21" s="57"/>
       <c r="D21" s="60"/>
@@ -7611,7 +7611,7 @@
       <c r="H21" s="48"/>
       <c r="I21" s="48"/>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="100"/>
       <c r="C22" s="57"/>
       <c r="D22" s="60"/>
@@ -7621,7 +7621,7 @@
       <c r="H22" s="48"/>
       <c r="I22" s="48"/>
     </row>
-    <row r="23" spans="2:9">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="100"/>
       <c r="C23" s="57"/>
       <c r="D23" s="60"/>
@@ -7631,7 +7631,7 @@
       <c r="H23" s="48"/>
       <c r="I23" s="48"/>
     </row>
-    <row r="24" spans="2:9">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" s="100"/>
       <c r="C24" s="83"/>
       <c r="D24" s="60"/>
@@ -7641,7 +7641,7 @@
       <c r="H24" s="48"/>
       <c r="I24" s="48"/>
     </row>
-    <row r="25" spans="2:9">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="100"/>
       <c r="C25" s="83"/>
       <c r="D25" s="60"/>
@@ -7651,7 +7651,7 @@
       <c r="H25" s="48"/>
       <c r="I25" s="48"/>
     </row>
-    <row r="26" spans="2:9">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="100"/>
       <c r="C26" s="83"/>
       <c r="D26" s="60"/>
@@ -7661,7 +7661,7 @@
       <c r="H26" s="48"/>
       <c r="I26" s="48"/>
     </row>
-    <row r="27" spans="2:9">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" s="100"/>
       <c r="C27" s="83"/>
       <c r="D27" s="60"/>
@@ -7671,7 +7671,7 @@
       <c r="H27" s="48"/>
       <c r="I27" s="48"/>
     </row>
-    <row r="28" spans="2:9">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" s="100"/>
       <c r="C28" s="83"/>
       <c r="D28" s="60"/>
@@ -7681,7 +7681,7 @@
       <c r="H28" s="48"/>
       <c r="I28" s="48"/>
     </row>
-    <row r="29" spans="2:9">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" s="100"/>
       <c r="C29" s="57"/>
       <c r="D29" s="60"/>
@@ -7702,22 +7702,22 @@
     <mergeCell ref="H5:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="I6:I25">
-    <cfRule type="cellIs" dxfId="9" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="27" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H29">
-    <cfRule type="cellIs" dxfId="8" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="26" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26:I29">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="6" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="8"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7733,7 +7733,7 @@
       <selection activeCell="B6" sqref="B6:E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
     <col min="2" max="2" width="21" style="1" customWidth="1"/>
@@ -7743,7 +7743,7 @@
     <col min="6" max="6" width="27.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="18">
+    <row r="2" spans="2:5" ht="18" x14ac:dyDescent="0.3">
       <c r="B2" s="63"/>
       <c r="C2" s="63"/>
       <c r="D2" s="101" t="s">
@@ -7751,19 +7751,19 @@
       </c>
       <c r="E2" s="101"/>
     </row>
-    <row r="3" spans="2:5" ht="18">
+    <row r="3" spans="2:5" ht="18" x14ac:dyDescent="0.3">
       <c r="B3" s="63"/>
       <c r="C3" s="63"/>
       <c r="D3" s="101"/>
       <c r="E3" s="101"/>
     </row>
-    <row r="4" spans="2:5" ht="18">
+    <row r="4" spans="2:5" ht="18" x14ac:dyDescent="0.3">
       <c r="B4" s="63"/>
       <c r="C4" s="63"/>
       <c r="D4" s="101"/>
       <c r="E4" s="101"/>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="55" t="s">
         <v>66</v>
       </c>
@@ -7777,214 +7777,214 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="15" customHeight="1">
+    <row r="6" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="64"/>
       <c r="C6" s="65"/>
       <c r="D6" s="43"/>
       <c r="E6" s="67"/>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="64"/>
       <c r="C7" s="65"/>
       <c r="D7" s="43"/>
       <c r="E7" s="67"/>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="64"/>
       <c r="C8" s="65"/>
       <c r="D8" s="43"/>
       <c r="E8" s="67"/>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="64"/>
       <c r="C9" s="65"/>
       <c r="D9" s="43"/>
       <c r="E9" s="67"/>
     </row>
-    <row r="10" spans="2:5">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="64"/>
       <c r="C10" s="65"/>
       <c r="D10" s="43"/>
       <c r="E10" s="67"/>
     </row>
-    <row r="11" spans="2:5">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" s="65"/>
       <c r="C11" s="65"/>
       <c r="D11" s="43"/>
       <c r="E11" s="47"/>
     </row>
-    <row r="12" spans="2:5">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="65"/>
       <c r="C12" s="65"/>
       <c r="D12" s="43"/>
       <c r="E12" s="47"/>
     </row>
-    <row r="13" spans="2:5">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" s="65"/>
       <c r="C13" s="65"/>
       <c r="D13" s="43"/>
       <c r="E13" s="47"/>
     </row>
-    <row r="14" spans="2:5">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" s="65"/>
       <c r="C14" s="65"/>
       <c r="D14" s="43"/>
       <c r="E14" s="47"/>
     </row>
-    <row r="15" spans="2:5">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" s="65"/>
       <c r="C15" s="65"/>
       <c r="D15" s="43"/>
       <c r="E15" s="47"/>
     </row>
-    <row r="16" spans="2:5">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B16" s="65"/>
       <c r="C16" s="65"/>
       <c r="D16" s="43"/>
       <c r="E16" s="47"/>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="65"/>
       <c r="C17" s="65"/>
       <c r="D17" s="43"/>
       <c r="E17" s="47"/>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="65"/>
       <c r="C18" s="65"/>
       <c r="D18" s="43"/>
       <c r="E18" s="47"/>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="65"/>
       <c r="C19" s="65"/>
       <c r="D19" s="43"/>
       <c r="E19" s="47"/>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="65"/>
       <c r="C20" s="65"/>
       <c r="D20" s="43"/>
       <c r="E20" s="47"/>
     </row>
-    <row r="21" spans="2:5" ht="15.75" customHeight="1">
+    <row r="21" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="65"/>
       <c r="C21" s="65"/>
       <c r="D21" s="43"/>
       <c r="E21" s="47"/>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="65"/>
       <c r="C22" s="65"/>
       <c r="D22" s="43"/>
       <c r="E22" s="47"/>
     </row>
-    <row r="23" spans="2:5" ht="15" customHeight="1">
+    <row r="23" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="65"/>
       <c r="C23" s="66"/>
       <c r="D23" s="44"/>
       <c r="E23" s="47"/>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="65"/>
       <c r="C24" s="66"/>
       <c r="D24" s="44"/>
       <c r="E24" s="47"/>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="65"/>
       <c r="C25" s="66"/>
       <c r="D25" s="44"/>
       <c r="E25" s="47"/>
     </row>
-    <row r="26" spans="2:5">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="65"/>
       <c r="C26" s="66"/>
       <c r="D26" s="44"/>
       <c r="E26" s="47"/>
     </row>
-    <row r="27" spans="2:5">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="65"/>
       <c r="C27" s="66"/>
       <c r="D27" s="44"/>
       <c r="E27" s="47"/>
     </row>
-    <row r="28" spans="2:5">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="65"/>
       <c r="C28" s="66"/>
       <c r="D28" s="44"/>
       <c r="E28" s="47"/>
     </row>
-    <row r="29" spans="2:5">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="65"/>
       <c r="C29" s="66"/>
       <c r="D29" s="44"/>
       <c r="E29" s="47"/>
     </row>
-    <row r="30" spans="2:5">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="65"/>
       <c r="C30" s="66"/>
       <c r="D30" s="44"/>
       <c r="E30" s="47"/>
     </row>
-    <row r="31" spans="2:5">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" s="65"/>
       <c r="C31" s="66"/>
       <c r="D31" s="44"/>
       <c r="E31" s="47"/>
     </row>
-    <row r="32" spans="2:5">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" s="65"/>
       <c r="C32" s="66"/>
       <c r="D32" s="44"/>
       <c r="E32" s="47"/>
     </row>
-    <row r="33" spans="2:5">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" s="65"/>
       <c r="C33" s="66"/>
       <c r="D33" s="44"/>
       <c r="E33" s="47"/>
     </row>
-    <row r="34" spans="2:5">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="65"/>
       <c r="C34" s="66"/>
       <c r="D34" s="44"/>
       <c r="E34" s="47"/>
     </row>
-    <row r="35" spans="2:5">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="65"/>
       <c r="C35" s="66"/>
       <c r="D35" s="44"/>
       <c r="E35" s="47"/>
     </row>
-    <row r="36" spans="2:5">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" s="65"/>
       <c r="C36" s="66"/>
       <c r="D36" s="44"/>
       <c r="E36" s="47"/>
     </row>
-    <row r="37" spans="2:5">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" s="65"/>
       <c r="C37" s="66"/>
       <c r="D37" s="44"/>
       <c r="E37" s="47"/>
     </row>
-    <row r="38" spans="2:5">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" s="65"/>
       <c r="C38" s="66"/>
       <c r="D38" s="44"/>
       <c r="E38" s="47"/>
     </row>
-    <row r="39" spans="2:5">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" s="65"/>
       <c r="C39" s="66"/>
       <c r="D39" s="44"/>
       <c r="E39" s="47"/>
     </row>
-    <row r="40" spans="2:5">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" s="65"/>
     </row>
-    <row r="41" spans="2:5">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B41" s="65"/>
     </row>
   </sheetData>
@@ -8007,7 +8007,7 @@
       <selection activeCell="U42" sqref="U42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="1.5546875" customWidth="1"/>
     <col min="3" max="3" width="2.109375" customWidth="1"/>
@@ -8023,7 +8023,7 @@
     <col min="17" max="17" width="1.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="6.75" customHeight="1" thickBot="1">
+    <row r="2" spans="2:16" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -8039,18 +8039,18 @@
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
     </row>
-    <row r="3" spans="2:16" ht="32.25" customHeight="1">
+    <row r="3" spans="2:16" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
-      <c r="D3" s="105" t="s">
+      <c r="D3" s="115" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="105"/>
-      <c r="I3" s="105"/>
-      <c r="J3" s="105"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="115"/>
+      <c r="I3" s="115"/>
+      <c r="J3" s="115"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
@@ -8058,12 +8058,12 @@
       <c r="O3" s="9"/>
       <c r="P3" s="10"/>
     </row>
-    <row r="4" spans="2:16">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" s="7"/>
       <c r="C4" s="11"/>
       <c r="P4" s="7"/>
     </row>
-    <row r="5" spans="2:16">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="7"/>
       <c r="C5" s="11"/>
       <c r="D5" s="12" t="s">
@@ -8071,19 +8071,19 @@
       </c>
       <c r="E5" s="32" t="str">
         <f ca="1">TEXT(E6,"ddd")</f>
-        <v>lun</v>
+        <v>mar</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="106" t="s">
+      <c r="G5" s="116" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="106"/>
+      <c r="H5" s="116"/>
       <c r="I5" s="13">
         <v>58</v>
       </c>
       <c r="P5" s="7"/>
     </row>
-    <row r="6" spans="2:16">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="7"/>
       <c r="C6" s="11"/>
       <c r="D6" s="12" t="s">
@@ -8091,22 +8091,22 @@
       </c>
       <c r="E6" s="32">
         <f ca="1">TODAY()</f>
-        <v>45495</v>
+        <v>45496</v>
       </c>
       <c r="F6" s="14"/>
-      <c r="G6" s="106" t="s">
+      <c r="G6" s="116" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="106"/>
+      <c r="H6" s="116"/>
       <c r="I6" s="13"/>
       <c r="P6" s="7"/>
     </row>
-    <row r="7" spans="2:16">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="7"/>
       <c r="C7" s="11"/>
       <c r="P7" s="7"/>
     </row>
-    <row r="8" spans="2:16" ht="35.25" customHeight="1">
+    <row r="8" spans="2:16" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7"/>
       <c r="C8" s="11"/>
       <c r="D8" s="15"/>
@@ -8127,7 +8127,7 @@
       <c r="O8" s="18"/>
       <c r="P8" s="7"/>
     </row>
-    <row r="9" spans="2:16" ht="6" customHeight="1">
+    <row r="9" spans="2:16" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="7"/>
       <c r="C9" s="11"/>
       <c r="D9" s="19"/>
@@ -8135,75 +8135,75 @@
       <c r="O9" s="21"/>
       <c r="P9" s="7"/>
     </row>
-    <row r="10" spans="2:16">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" s="7"/>
       <c r="C10" s="11"/>
       <c r="D10" s="19"/>
-      <c r="L10" s="107">
+      <c r="L10" s="117">
         <f>I6/I5</f>
         <v>0</v>
       </c>
-      <c r="N10" s="107"/>
+      <c r="N10" s="117"/>
       <c r="O10" s="21"/>
       <c r="P10" s="7"/>
     </row>
-    <row r="11" spans="2:16">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" s="7"/>
       <c r="C11" s="11"/>
       <c r="D11" s="19"/>
-      <c r="L11" s="107"/>
-      <c r="N11" s="107"/>
+      <c r="L11" s="117"/>
+      <c r="N11" s="117"/>
       <c r="O11" s="21"/>
       <c r="P11" s="7"/>
     </row>
-    <row r="12" spans="2:16" ht="3.75" customHeight="1">
+    <row r="12" spans="2:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
       <c r="C12" s="11"/>
       <c r="D12" s="19"/>
       <c r="O12" s="21"/>
       <c r="P12" s="7"/>
     </row>
-    <row r="13" spans="2:16">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13" s="7"/>
       <c r="C13" s="11"/>
       <c r="D13" s="19"/>
-      <c r="L13" s="103" t="s">
+      <c r="L13" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M13" s="103"/>
-      <c r="N13" s="103"/>
+      <c r="M13" s="114"/>
+      <c r="N13" s="114"/>
       <c r="O13" s="21"/>
       <c r="P13" s="7"/>
     </row>
-    <row r="14" spans="2:16">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14" s="7"/>
       <c r="C14" s="11"/>
       <c r="D14" s="19"/>
       <c r="O14" s="21"/>
       <c r="P14" s="7"/>
     </row>
-    <row r="15" spans="2:16">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15" s="7"/>
       <c r="C15" s="11"/>
       <c r="D15" s="19"/>
       <c r="O15" s="21"/>
       <c r="P15" s="7"/>
     </row>
-    <row r="16" spans="2:16">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B16" s="7"/>
       <c r="C16" s="11"/>
       <c r="D16" s="19"/>
       <c r="O16" s="21"/>
       <c r="P16" s="7"/>
     </row>
-    <row r="17" spans="2:16">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B17" s="7"/>
       <c r="C17" s="11"/>
       <c r="D17" s="19"/>
       <c r="O17" s="21"/>
       <c r="P17" s="7"/>
     </row>
-    <row r="18" spans="2:16">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B18" s="7"/>
       <c r="C18" s="11"/>
       <c r="D18" s="22"/>
@@ -8220,7 +8220,7 @@
       <c r="O18" s="24"/>
       <c r="P18" s="7"/>
     </row>
-    <row r="19" spans="2:16" ht="21" customHeight="1">
+    <row r="19" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="7"/>
       <c r="C19" s="11"/>
       <c r="D19" s="69"/>
@@ -8237,7 +8237,7 @@
       <c r="O19" s="69"/>
       <c r="P19" s="7"/>
     </row>
-    <row r="20" spans="2:16" ht="21" customHeight="1" thickBot="1">
+    <row r="20" spans="2:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="7"/>
       <c r="C20" s="11"/>
       <c r="D20" s="70" t="s">
@@ -8256,17 +8256,17 @@
       <c r="O20" s="69"/>
       <c r="P20" s="7"/>
     </row>
-    <row r="21" spans="2:16" s="75" customFormat="1" ht="18">
+    <row r="21" spans="2:16" s="75" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B21" s="76"/>
       <c r="C21" s="77"/>
       <c r="D21" s="72"/>
-      <c r="E21" s="108" t="s">
+      <c r="E21" s="112" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="108"/>
-      <c r="G21" s="108"/>
-      <c r="H21" s="108"/>
-      <c r="I21" s="108"/>
+      <c r="F21" s="112"/>
+      <c r="G21" s="112"/>
+      <c r="H21" s="112"/>
+      <c r="I21" s="112"/>
       <c r="J21" s="72" t="s">
         <v>75</v>
       </c>
@@ -8277,17 +8277,17 @@
       <c r="O21" s="78"/>
       <c r="P21" s="76"/>
     </row>
-    <row r="22" spans="2:16" ht="24.75" customHeight="1">
+    <row r="22" spans="2:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="7"/>
       <c r="C22" s="11"/>
       <c r="D22" s="74">
         <v>1</v>
       </c>
-      <c r="E22" s="109"/>
-      <c r="F22" s="109"/>
-      <c r="G22" s="109"/>
-      <c r="H22" s="109"/>
-      <c r="I22" s="109"/>
+      <c r="E22" s="110"/>
+      <c r="F22" s="110"/>
+      <c r="G22" s="110"/>
+      <c r="H22" s="110"/>
+      <c r="I22" s="110"/>
       <c r="J22" s="97"/>
       <c r="K22" s="97"/>
       <c r="L22" s="97"/>
@@ -8296,17 +8296,17 @@
       <c r="O22" s="69"/>
       <c r="P22" s="7"/>
     </row>
-    <row r="23" spans="2:16" ht="24.75" customHeight="1">
+    <row r="23" spans="2:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="7"/>
       <c r="C23" s="11"/>
       <c r="D23" s="74">
         <v>2</v>
       </c>
-      <c r="E23" s="109"/>
-      <c r="F23" s="109"/>
-      <c r="G23" s="109"/>
-      <c r="H23" s="109"/>
-      <c r="I23" s="109"/>
+      <c r="E23" s="110"/>
+      <c r="F23" s="110"/>
+      <c r="G23" s="110"/>
+      <c r="H23" s="110"/>
+      <c r="I23" s="110"/>
       <c r="J23" s="97"/>
       <c r="K23" s="97"/>
       <c r="L23" s="97"/>
@@ -8315,17 +8315,17 @@
       <c r="O23" s="69"/>
       <c r="P23" s="7"/>
     </row>
-    <row r="24" spans="2:16" ht="24.75" customHeight="1">
+    <row r="24" spans="2:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="7"/>
       <c r="C24" s="11"/>
       <c r="D24" s="74">
         <v>3</v>
       </c>
-      <c r="E24" s="109"/>
-      <c r="F24" s="109"/>
-      <c r="G24" s="109"/>
-      <c r="H24" s="109"/>
-      <c r="I24" s="109"/>
+      <c r="E24" s="110"/>
+      <c r="F24" s="110"/>
+      <c r="G24" s="110"/>
+      <c r="H24" s="110"/>
+      <c r="I24" s="110"/>
       <c r="J24" s="97"/>
       <c r="K24" s="97"/>
       <c r="L24" s="97"/>
@@ -8334,17 +8334,17 @@
       <c r="O24" s="69"/>
       <c r="P24" s="7"/>
     </row>
-    <row r="25" spans="2:16" ht="24.75" customHeight="1">
+    <row r="25" spans="2:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="7"/>
       <c r="C25" s="11"/>
       <c r="D25" s="74">
         <v>4</v>
       </c>
-      <c r="E25" s="109"/>
-      <c r="F25" s="109"/>
-      <c r="G25" s="109"/>
-      <c r="H25" s="109"/>
-      <c r="I25" s="109"/>
+      <c r="E25" s="110"/>
+      <c r="F25" s="110"/>
+      <c r="G25" s="110"/>
+      <c r="H25" s="110"/>
+      <c r="I25" s="110"/>
       <c r="J25" s="97"/>
       <c r="K25" s="97"/>
       <c r="L25" s="97"/>
@@ -8353,17 +8353,17 @@
       <c r="O25" s="69"/>
       <c r="P25" s="7"/>
     </row>
-    <row r="26" spans="2:16" ht="24.75" customHeight="1">
+    <row r="26" spans="2:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="7"/>
       <c r="C26" s="11"/>
       <c r="D26" s="74">
         <v>5</v>
       </c>
-      <c r="E26" s="109"/>
-      <c r="F26" s="109"/>
-      <c r="G26" s="109"/>
-      <c r="H26" s="109"/>
-      <c r="I26" s="109"/>
+      <c r="E26" s="110"/>
+      <c r="F26" s="110"/>
+      <c r="G26" s="110"/>
+      <c r="H26" s="110"/>
+      <c r="I26" s="110"/>
       <c r="J26" s="97"/>
       <c r="K26" s="97"/>
       <c r="L26" s="97"/>
@@ -8372,7 +8372,7 @@
       <c r="O26" s="69"/>
       <c r="P26" s="7"/>
     </row>
-    <row r="27" spans="2:16">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B27" s="7"/>
       <c r="C27" s="11"/>
       <c r="D27" s="69"/>
@@ -8389,7 +8389,7 @@
       <c r="O27" s="69"/>
       <c r="P27" s="7"/>
     </row>
-    <row r="28" spans="2:16" ht="21.6" thickBot="1">
+    <row r="28" spans="2:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B28" s="7"/>
       <c r="C28" s="11"/>
       <c r="D28" s="70" t="s">
@@ -8408,125 +8408,125 @@
       <c r="O28" s="69"/>
       <c r="P28" s="7"/>
     </row>
-    <row r="29" spans="2:16" ht="24" customHeight="1">
+    <row r="29" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="7"/>
       <c r="C29" s="11"/>
       <c r="D29" s="71"/>
-      <c r="E29" s="108" t="s">
+      <c r="E29" s="112" t="s">
         <v>14</v>
       </c>
-      <c r="F29" s="108"/>
-      <c r="G29" s="108"/>
-      <c r="H29" s="108"/>
-      <c r="I29" s="108"/>
+      <c r="F29" s="112"/>
+      <c r="G29" s="112"/>
+      <c r="H29" s="112"/>
+      <c r="I29" s="112"/>
       <c r="J29" s="72" t="s">
         <v>75</v>
       </c>
       <c r="K29" s="72"/>
-      <c r="L29" s="104" t="s">
+      <c r="L29" s="105" t="s">
         <v>76</v>
       </c>
-      <c r="M29" s="104"/>
-      <c r="N29" s="104"/>
+      <c r="M29" s="105"/>
+      <c r="N29" s="105"/>
       <c r="O29" s="69"/>
       <c r="P29" s="7"/>
     </row>
-    <row r="30" spans="2:16" ht="24.75" customHeight="1">
+    <row r="30" spans="2:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="7"/>
       <c r="C30" s="11"/>
       <c r="D30" s="74">
         <v>1</v>
       </c>
-      <c r="E30" s="109"/>
-      <c r="F30" s="109"/>
-      <c r="G30" s="109"/>
-      <c r="H30" s="109"/>
-      <c r="I30" s="109"/>
-      <c r="J30" s="109"/>
-      <c r="K30" s="109"/>
-      <c r="L30" s="113"/>
-      <c r="M30" s="113"/>
-      <c r="N30" s="113"/>
+      <c r="E30" s="110"/>
+      <c r="F30" s="110"/>
+      <c r="G30" s="110"/>
+      <c r="H30" s="110"/>
+      <c r="I30" s="110"/>
+      <c r="J30" s="110"/>
+      <c r="K30" s="110"/>
+      <c r="L30" s="111"/>
+      <c r="M30" s="111"/>
+      <c r="N30" s="111"/>
       <c r="O30" s="69"/>
       <c r="P30" s="7"/>
     </row>
-    <row r="31" spans="2:16" ht="24.75" customHeight="1">
+    <row r="31" spans="2:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="7"/>
       <c r="C31" s="11"/>
       <c r="D31" s="74">
         <v>2</v>
       </c>
-      <c r="E31" s="109"/>
-      <c r="F31" s="109"/>
-      <c r="G31" s="109"/>
-      <c r="H31" s="109"/>
-      <c r="I31" s="109"/>
-      <c r="J31" s="109"/>
-      <c r="K31" s="109"/>
-      <c r="L31" s="113"/>
-      <c r="M31" s="113"/>
-      <c r="N31" s="113"/>
+      <c r="E31" s="110"/>
+      <c r="F31" s="110"/>
+      <c r="G31" s="110"/>
+      <c r="H31" s="110"/>
+      <c r="I31" s="110"/>
+      <c r="J31" s="110"/>
+      <c r="K31" s="110"/>
+      <c r="L31" s="111"/>
+      <c r="M31" s="111"/>
+      <c r="N31" s="111"/>
       <c r="O31" s="69"/>
       <c r="P31" s="7"/>
     </row>
-    <row r="32" spans="2:16" ht="24.75" customHeight="1">
+    <row r="32" spans="2:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="7"/>
       <c r="C32" s="11"/>
       <c r="D32" s="74">
         <v>3</v>
       </c>
-      <c r="E32" s="109"/>
-      <c r="F32" s="109"/>
-      <c r="G32" s="109"/>
-      <c r="H32" s="109"/>
-      <c r="I32" s="109"/>
-      <c r="J32" s="109"/>
-      <c r="K32" s="109"/>
-      <c r="L32" s="113"/>
-      <c r="M32" s="113"/>
-      <c r="N32" s="113"/>
+      <c r="E32" s="110"/>
+      <c r="F32" s="110"/>
+      <c r="G32" s="110"/>
+      <c r="H32" s="110"/>
+      <c r="I32" s="110"/>
+      <c r="J32" s="110"/>
+      <c r="K32" s="110"/>
+      <c r="L32" s="111"/>
+      <c r="M32" s="111"/>
+      <c r="N32" s="111"/>
       <c r="O32" s="69"/>
       <c r="P32" s="7"/>
     </row>
-    <row r="33" spans="2:16" ht="24.75" customHeight="1">
+    <row r="33" spans="2:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="7"/>
       <c r="C33" s="11"/>
       <c r="D33" s="74">
         <v>4</v>
       </c>
-      <c r="E33" s="109"/>
-      <c r="F33" s="109"/>
-      <c r="G33" s="109"/>
-      <c r="H33" s="109"/>
-      <c r="I33" s="109"/>
-      <c r="J33" s="109"/>
-      <c r="K33" s="109"/>
-      <c r="L33" s="113"/>
-      <c r="M33" s="113"/>
-      <c r="N33" s="113"/>
+      <c r="E33" s="110"/>
+      <c r="F33" s="110"/>
+      <c r="G33" s="110"/>
+      <c r="H33" s="110"/>
+      <c r="I33" s="110"/>
+      <c r="J33" s="110"/>
+      <c r="K33" s="110"/>
+      <c r="L33" s="111"/>
+      <c r="M33" s="111"/>
+      <c r="N33" s="111"/>
       <c r="O33" s="69"/>
       <c r="P33" s="7"/>
     </row>
-    <row r="34" spans="2:16" ht="24.75" customHeight="1">
+    <row r="34" spans="2:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="7"/>
       <c r="C34" s="11"/>
       <c r="D34" s="74">
         <v>5</v>
       </c>
-      <c r="E34" s="109"/>
-      <c r="F34" s="109"/>
-      <c r="G34" s="109"/>
-      <c r="H34" s="109"/>
-      <c r="I34" s="109"/>
-      <c r="J34" s="109"/>
-      <c r="K34" s="109"/>
-      <c r="L34" s="113"/>
-      <c r="M34" s="113"/>
-      <c r="N34" s="113"/>
+      <c r="E34" s="110"/>
+      <c r="F34" s="110"/>
+      <c r="G34" s="110"/>
+      <c r="H34" s="110"/>
+      <c r="I34" s="110"/>
+      <c r="J34" s="110"/>
+      <c r="K34" s="110"/>
+      <c r="L34" s="111"/>
+      <c r="M34" s="111"/>
+      <c r="N34" s="111"/>
       <c r="O34" s="69"/>
       <c r="P34" s="7"/>
     </row>
-    <row r="35" spans="2:16">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B35" s="7"/>
       <c r="C35" s="11"/>
       <c r="D35" s="74"/>
@@ -8543,7 +8543,7 @@
       <c r="O35" s="69"/>
       <c r="P35" s="7"/>
     </row>
-    <row r="36" spans="2:16">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B36" s="7"/>
       <c r="C36" s="11"/>
       <c r="D36" s="69"/>
@@ -8560,7 +8560,7 @@
       <c r="O36" s="69"/>
       <c r="P36" s="7"/>
     </row>
-    <row r="37" spans="2:16" ht="21.6" thickBot="1">
+    <row r="37" spans="2:16" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B37" s="7"/>
       <c r="C37" s="11"/>
       <c r="D37" s="70" t="s">
@@ -8571,89 +8571,89 @@
       <c r="G37" s="69"/>
       <c r="H37" s="69"/>
       <c r="I37" s="69"/>
-      <c r="J37" s="116" t="s">
+      <c r="J37" s="109" t="s">
         <v>78</v>
       </c>
-      <c r="K37" s="116"/>
-      <c r="L37" s="114">
+      <c r="K37" s="109"/>
+      <c r="L37" s="107">
         <v>45440</v>
       </c>
-      <c r="M37" s="115"/>
-      <c r="N37" s="115"/>
+      <c r="M37" s="108"/>
+      <c r="N37" s="108"/>
       <c r="O37" s="69"/>
       <c r="P37" s="7"/>
     </row>
-    <row r="38" spans="2:16" s="75" customFormat="1" ht="18">
+    <row r="38" spans="2:16" s="75" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B38" s="76"/>
       <c r="C38" s="77"/>
       <c r="D38" s="72"/>
-      <c r="E38" s="117" t="s">
+      <c r="E38" s="106" t="s">
         <v>74</v>
       </c>
-      <c r="F38" s="117"/>
-      <c r="G38" s="117"/>
-      <c r="H38" s="117"/>
-      <c r="I38" s="117"/>
+      <c r="F38" s="106"/>
+      <c r="G38" s="106"/>
+      <c r="H38" s="106"/>
+      <c r="I38" s="106"/>
       <c r="J38" s="73" t="s">
         <v>3</v>
       </c>
       <c r="K38" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="L38" s="104" t="s">
+      <c r="L38" s="105" t="s">
         <v>75</v>
       </c>
-      <c r="M38" s="104"/>
-      <c r="N38" s="104"/>
+      <c r="M38" s="105"/>
+      <c r="N38" s="105"/>
       <c r="O38" s="78"/>
       <c r="P38" s="76"/>
     </row>
-    <row r="39" spans="2:16" ht="22.5" customHeight="1">
+    <row r="39" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="7"/>
       <c r="C39" s="11"/>
       <c r="D39" s="74">
         <v>1</v>
       </c>
-      <c r="E39" s="110" t="s">
+      <c r="E39" s="104" t="s">
         <v>33</v>
       </c>
-      <c r="F39" s="110"/>
-      <c r="G39" s="110"/>
-      <c r="H39" s="110"/>
-      <c r="I39" s="110"/>
+      <c r="F39" s="104"/>
+      <c r="G39" s="104"/>
+      <c r="H39" s="104"/>
+      <c r="I39" s="104"/>
       <c r="J39" s="56">
         <v>1</v>
       </c>
       <c r="K39" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="L39" s="111" t="s">
+      <c r="L39" s="113" t="s">
         <v>79</v>
       </c>
-      <c r="M39" s="111"/>
-      <c r="N39" s="111"/>
+      <c r="M39" s="113"/>
+      <c r="N39" s="113"/>
       <c r="O39" s="69"/>
       <c r="P39" s="7"/>
     </row>
-    <row r="40" spans="2:16" ht="22.5" customHeight="1">
+    <row r="40" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="7"/>
       <c r="C40" s="11"/>
       <c r="D40" s="74">
         <v>2</v>
       </c>
-      <c r="E40" s="110" t="s">
+      <c r="E40" s="104" t="s">
         <v>42</v>
       </c>
-      <c r="F40" s="110" t="s">
+      <c r="F40" s="104" t="s">
         <v>42</v>
       </c>
-      <c r="G40" s="110" t="s">
+      <c r="G40" s="104" t="s">
         <v>42</v>
       </c>
-      <c r="H40" s="110" t="s">
+      <c r="H40" s="104" t="s">
         <v>42</v>
       </c>
-      <c r="I40" s="110" t="s">
+      <c r="I40" s="104" t="s">
         <v>42</v>
       </c>
       <c r="J40" s="56">
@@ -8662,33 +8662,33 @@
       <c r="K40" s="79" t="s">
         <v>43</v>
       </c>
-      <c r="L40" s="112" t="s">
+      <c r="L40" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="M40" s="112"/>
-      <c r="N40" s="112"/>
+      <c r="M40" s="103"/>
+      <c r="N40" s="103"/>
       <c r="O40" s="69"/>
       <c r="P40" s="7"/>
     </row>
-    <row r="41" spans="2:16" ht="22.5" customHeight="1">
+    <row r="41" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="7"/>
       <c r="C41" s="11"/>
       <c r="D41" s="74">
         <v>3</v>
       </c>
-      <c r="E41" s="110" t="s">
+      <c r="E41" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="F41" s="110" t="s">
+      <c r="F41" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="G41" s="110" t="s">
+      <c r="G41" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="H41" s="110" t="s">
+      <c r="H41" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="I41" s="110" t="s">
+      <c r="I41" s="104" t="s">
         <v>44</v>
       </c>
       <c r="J41" s="56">
@@ -8697,33 +8697,33 @@
       <c r="K41" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="L41" s="112" t="s">
+      <c r="L41" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="M41" s="112"/>
-      <c r="N41" s="112"/>
+      <c r="M41" s="103"/>
+      <c r="N41" s="103"/>
       <c r="O41" s="69"/>
       <c r="P41" s="7"/>
     </row>
-    <row r="42" spans="2:16" ht="22.5" customHeight="1">
+    <row r="42" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="7"/>
       <c r="C42" s="11"/>
       <c r="D42" s="74">
         <v>4</v>
       </c>
-      <c r="E42" s="110" t="s">
+      <c r="E42" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="F42" s="110" t="s">
+      <c r="F42" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="G42" s="110" t="s">
+      <c r="G42" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="H42" s="110" t="s">
+      <c r="H42" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="I42" s="110" t="s">
+      <c r="I42" s="104" t="s">
         <v>26</v>
       </c>
       <c r="J42" s="56">
@@ -8732,33 +8732,33 @@
       <c r="K42" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="L42" s="112" t="s">
+      <c r="L42" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="M42" s="112"/>
-      <c r="N42" s="112"/>
+      <c r="M42" s="103"/>
+      <c r="N42" s="103"/>
       <c r="O42" s="69"/>
       <c r="P42" s="7"/>
     </row>
-    <row r="43" spans="2:16" ht="22.5" customHeight="1">
+    <row r="43" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="7"/>
       <c r="C43" s="11"/>
       <c r="D43" s="74">
         <v>5</v>
       </c>
-      <c r="E43" s="110" t="s">
+      <c r="E43" s="104" t="s">
         <v>46</v>
       </c>
-      <c r="F43" s="110" t="s">
+      <c r="F43" s="104" t="s">
         <v>46</v>
       </c>
-      <c r="G43" s="110" t="s">
+      <c r="G43" s="104" t="s">
         <v>46</v>
       </c>
-      <c r="H43" s="110" t="s">
+      <c r="H43" s="104" t="s">
         <v>46</v>
       </c>
-      <c r="I43" s="110" t="s">
+      <c r="I43" s="104" t="s">
         <v>46</v>
       </c>
       <c r="J43" s="56">
@@ -8767,33 +8767,33 @@
       <c r="K43" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="L43" s="112" t="s">
+      <c r="L43" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="M43" s="112"/>
-      <c r="N43" s="112"/>
+      <c r="M43" s="103"/>
+      <c r="N43" s="103"/>
       <c r="O43" s="69"/>
       <c r="P43" s="7"/>
     </row>
-    <row r="44" spans="2:16" ht="22.5" customHeight="1">
+    <row r="44" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="7"/>
       <c r="C44" s="11"/>
       <c r="D44" s="74">
         <v>6</v>
       </c>
-      <c r="E44" s="110" t="s">
+      <c r="E44" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="F44" s="110" t="s">
+      <c r="F44" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="G44" s="110" t="s">
+      <c r="G44" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="H44" s="110" t="s">
+      <c r="H44" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="I44" s="110" t="s">
+      <c r="I44" s="104" t="s">
         <v>26</v>
       </c>
       <c r="J44" s="56">
@@ -8802,33 +8802,33 @@
       <c r="K44" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="L44" s="112" t="s">
+      <c r="L44" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="M44" s="112"/>
-      <c r="N44" s="112"/>
+      <c r="M44" s="103"/>
+      <c r="N44" s="103"/>
       <c r="O44" s="69"/>
       <c r="P44" s="7"/>
     </row>
-    <row r="45" spans="2:16" ht="22.5" customHeight="1">
+    <row r="45" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="7"/>
       <c r="C45" s="11"/>
       <c r="D45" s="74">
         <v>7</v>
       </c>
-      <c r="E45" s="110" t="s">
+      <c r="E45" s="104" t="s">
         <v>29</v>
       </c>
-      <c r="F45" s="110" t="s">
+      <c r="F45" s="104" t="s">
         <v>29</v>
       </c>
-      <c r="G45" s="110" t="s">
+      <c r="G45" s="104" t="s">
         <v>29</v>
       </c>
-      <c r="H45" s="110" t="s">
+      <c r="H45" s="104" t="s">
         <v>29</v>
       </c>
-      <c r="I45" s="110" t="s">
+      <c r="I45" s="104" t="s">
         <v>29</v>
       </c>
       <c r="J45" s="56">
@@ -8837,33 +8837,33 @@
       <c r="K45" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="L45" s="112" t="s">
+      <c r="L45" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="M45" s="112"/>
-      <c r="N45" s="112"/>
+      <c r="M45" s="103"/>
+      <c r="N45" s="103"/>
       <c r="O45" s="69"/>
       <c r="P45" s="7"/>
     </row>
-    <row r="46" spans="2:16" ht="22.5" customHeight="1">
+    <row r="46" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="7"/>
       <c r="C46" s="11"/>
       <c r="D46" s="74">
         <v>8</v>
       </c>
-      <c r="E46" s="110" t="s">
+      <c r="E46" s="104" t="s">
         <v>49</v>
       </c>
-      <c r="F46" s="110" t="s">
+      <c r="F46" s="104" t="s">
         <v>49</v>
       </c>
-      <c r="G46" s="110" t="s">
+      <c r="G46" s="104" t="s">
         <v>49</v>
       </c>
-      <c r="H46" s="110" t="s">
+      <c r="H46" s="104" t="s">
         <v>49</v>
       </c>
-      <c r="I46" s="110" t="s">
+      <c r="I46" s="104" t="s">
         <v>49</v>
       </c>
       <c r="J46" s="56">
@@ -8872,33 +8872,33 @@
       <c r="K46" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="L46" s="112" t="s">
+      <c r="L46" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="M46" s="112"/>
-      <c r="N46" s="112"/>
+      <c r="M46" s="103"/>
+      <c r="N46" s="103"/>
       <c r="O46" s="69"/>
       <c r="P46" s="7"/>
     </row>
-    <row r="47" spans="2:16" ht="22.5" customHeight="1">
+    <row r="47" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="7"/>
       <c r="C47" s="11"/>
       <c r="D47" s="74">
         <v>9</v>
       </c>
-      <c r="E47" s="110" t="s">
+      <c r="E47" s="104" t="s">
         <v>51</v>
       </c>
-      <c r="F47" s="110" t="s">
+      <c r="F47" s="104" t="s">
         <v>51</v>
       </c>
-      <c r="G47" s="110" t="s">
+      <c r="G47" s="104" t="s">
         <v>51</v>
       </c>
-      <c r="H47" s="110" t="s">
+      <c r="H47" s="104" t="s">
         <v>51</v>
       </c>
-      <c r="I47" s="110" t="s">
+      <c r="I47" s="104" t="s">
         <v>51</v>
       </c>
       <c r="J47" s="56">
@@ -8907,33 +8907,33 @@
       <c r="K47" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="L47" s="112" t="s">
+      <c r="L47" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="M47" s="112"/>
-      <c r="N47" s="112"/>
+      <c r="M47" s="103"/>
+      <c r="N47" s="103"/>
       <c r="O47" s="69"/>
       <c r="P47" s="7"/>
     </row>
-    <row r="48" spans="2:16" ht="22.5" customHeight="1">
+    <row r="48" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="7"/>
       <c r="C48" s="11"/>
       <c r="D48" s="74">
         <v>10</v>
       </c>
-      <c r="E48" s="110" t="s">
+      <c r="E48" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="F48" s="110" t="s">
+      <c r="F48" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="G48" s="110" t="s">
+      <c r="G48" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="H48" s="110" t="s">
+      <c r="H48" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="I48" s="110" t="s">
+      <c r="I48" s="104" t="s">
         <v>30</v>
       </c>
       <c r="J48" s="56">
@@ -8942,33 +8942,33 @@
       <c r="K48" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="L48" s="112" t="s">
+      <c r="L48" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="M48" s="112"/>
-      <c r="N48" s="112"/>
+      <c r="M48" s="103"/>
+      <c r="N48" s="103"/>
       <c r="O48" s="69"/>
       <c r="P48" s="7"/>
     </row>
-    <row r="49" spans="2:16" ht="22.5" customHeight="1">
+    <row r="49" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="7"/>
       <c r="C49" s="11"/>
       <c r="D49" s="74">
         <v>11</v>
       </c>
-      <c r="E49" s="110" t="s">
+      <c r="E49" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="F49" s="110" t="s">
+      <c r="F49" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="G49" s="110" t="s">
+      <c r="G49" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="H49" s="110" t="s">
+      <c r="H49" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="I49" s="110" t="s">
+      <c r="I49" s="104" t="s">
         <v>26</v>
       </c>
       <c r="J49" s="56">
@@ -8977,33 +8977,33 @@
       <c r="K49" s="79" t="s">
         <v>54</v>
       </c>
-      <c r="L49" s="112" t="s">
+      <c r="L49" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="M49" s="112"/>
-      <c r="N49" s="112"/>
+      <c r="M49" s="103"/>
+      <c r="N49" s="103"/>
       <c r="O49" s="69"/>
       <c r="P49" s="7"/>
     </row>
-    <row r="50" spans="2:16" ht="22.5" customHeight="1">
+    <row r="50" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="7"/>
       <c r="C50" s="11"/>
       <c r="D50" s="74">
         <v>12</v>
       </c>
-      <c r="E50" s="110" t="s">
+      <c r="E50" s="104" t="s">
         <v>29</v>
       </c>
-      <c r="F50" s="110" t="s">
+      <c r="F50" s="104" t="s">
         <v>29</v>
       </c>
-      <c r="G50" s="110" t="s">
+      <c r="G50" s="104" t="s">
         <v>29</v>
       </c>
-      <c r="H50" s="110" t="s">
+      <c r="H50" s="104" t="s">
         <v>29</v>
       </c>
-      <c r="I50" s="110" t="s">
+      <c r="I50" s="104" t="s">
         <v>29</v>
       </c>
       <c r="J50" s="56">
@@ -9012,33 +9012,33 @@
       <c r="K50" s="79" t="s">
         <v>55</v>
       </c>
-      <c r="L50" s="112" t="s">
+      <c r="L50" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="M50" s="112"/>
-      <c r="N50" s="112"/>
+      <c r="M50" s="103"/>
+      <c r="N50" s="103"/>
       <c r="O50" s="69"/>
       <c r="P50" s="7"/>
     </row>
-    <row r="51" spans="2:16" ht="22.5" customHeight="1">
+    <row r="51" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="7"/>
       <c r="C51" s="11"/>
       <c r="D51" s="74">
         <v>13</v>
       </c>
-      <c r="E51" s="110" t="s">
+      <c r="E51" s="104" t="s">
         <v>57</v>
       </c>
-      <c r="F51" s="110" t="s">
+      <c r="F51" s="104" t="s">
         <v>57</v>
       </c>
-      <c r="G51" s="110" t="s">
+      <c r="G51" s="104" t="s">
         <v>57</v>
       </c>
-      <c r="H51" s="110" t="s">
+      <c r="H51" s="104" t="s">
         <v>57</v>
       </c>
-      <c r="I51" s="110" t="s">
+      <c r="I51" s="104" t="s">
         <v>57</v>
       </c>
       <c r="J51" s="56" t="s">
@@ -9047,33 +9047,33 @@
       <c r="K51" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="L51" s="112" t="s">
+      <c r="L51" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="M51" s="112"/>
-      <c r="N51" s="112"/>
+      <c r="M51" s="103"/>
+      <c r="N51" s="103"/>
       <c r="O51" s="69"/>
       <c r="P51" s="7"/>
     </row>
-    <row r="52" spans="2:16" ht="22.5" customHeight="1">
+    <row r="52" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="7"/>
       <c r="C52" s="11"/>
       <c r="D52" s="74">
         <v>14</v>
       </c>
-      <c r="E52" s="110" t="s">
+      <c r="E52" s="104" t="s">
         <v>56</v>
       </c>
-      <c r="F52" s="110" t="s">
+      <c r="F52" s="104" t="s">
         <v>56</v>
       </c>
-      <c r="G52" s="110" t="s">
+      <c r="G52" s="104" t="s">
         <v>56</v>
       </c>
-      <c r="H52" s="110" t="s">
+      <c r="H52" s="104" t="s">
         <v>56</v>
       </c>
-      <c r="I52" s="110" t="s">
+      <c r="I52" s="104" t="s">
         <v>56</v>
       </c>
       <c r="J52" s="56">
@@ -9082,33 +9082,33 @@
       <c r="K52" s="79" t="s">
         <v>59</v>
       </c>
-      <c r="L52" s="112" t="s">
+      <c r="L52" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="M52" s="112"/>
-      <c r="N52" s="112"/>
+      <c r="M52" s="103"/>
+      <c r="N52" s="103"/>
       <c r="O52" s="69"/>
       <c r="P52" s="7"/>
     </row>
-    <row r="53" spans="2:16" ht="22.5" customHeight="1">
+    <row r="53" spans="2:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="7"/>
       <c r="C53" s="11"/>
       <c r="D53" s="74">
         <v>15</v>
       </c>
-      <c r="E53" s="110" t="s">
+      <c r="E53" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="F53" s="110" t="s">
+      <c r="F53" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="G53" s="110" t="s">
+      <c r="G53" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="H53" s="110" t="s">
+      <c r="H53" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="I53" s="110" t="s">
+      <c r="I53" s="104" t="s">
         <v>27</v>
       </c>
       <c r="J53" s="56">
@@ -9117,15 +9117,15 @@
       <c r="K53" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="L53" s="112" t="s">
+      <c r="L53" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="M53" s="112"/>
-      <c r="N53" s="112"/>
+      <c r="M53" s="103"/>
+      <c r="N53" s="103"/>
       <c r="O53" s="69"/>
       <c r="P53" s="7"/>
     </row>
-    <row r="54" spans="2:16" ht="9" customHeight="1" thickBot="1">
+    <row r="54" spans="2:16" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B54" s="7"/>
       <c r="C54" s="25"/>
       <c r="D54" s="6"/>
@@ -9142,12 +9142,12 @@
       <c r="O54" s="6"/>
       <c r="P54" s="26"/>
     </row>
-    <row r="55" spans="2:16" ht="6.75" customHeight="1"/>
-    <row r="56" spans="2:16" ht="32.25" customHeight="1"/>
-    <row r="61" spans="2:16" ht="35.25" customHeight="1"/>
-    <row r="62" spans="2:16" ht="6" customHeight="1"/>
-    <row r="65" spans="11:18" ht="3.75" customHeight="1"/>
-    <row r="66" spans="11:18">
+    <row r="55" spans="2:16" ht="6.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="2:16" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="2:16" ht="35.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="2:16" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="65" spans="11:18" ht="3.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="11:18" x14ac:dyDescent="0.3">
       <c r="K66" s="68"/>
       <c r="L66" s="68"/>
       <c r="M66" s="68"/>
@@ -9157,7 +9157,7 @@
       <c r="Q66" s="68"/>
       <c r="R66" s="68"/>
     </row>
-    <row r="67" spans="11:18">
+    <row r="67" spans="11:18" x14ac:dyDescent="0.3">
       <c r="K67" s="68"/>
       <c r="L67" s="68"/>
       <c r="M67" s="68"/>
@@ -9167,7 +9167,7 @@
       <c r="Q67" s="68"/>
       <c r="R67" s="68"/>
     </row>
-    <row r="68" spans="11:18">
+    <row r="68" spans="11:18" x14ac:dyDescent="0.3">
       <c r="K68" s="68"/>
       <c r="L68" s="68"/>
       <c r="M68" s="68"/>
@@ -9177,7 +9177,7 @@
       <c r="Q68" s="68"/>
       <c r="R68" s="68"/>
     </row>
-    <row r="69" spans="11:18">
+    <row r="69" spans="11:18" x14ac:dyDescent="0.3">
       <c r="K69" s="68"/>
       <c r="L69" s="68"/>
       <c r="M69" s="68"/>
@@ -9187,7 +9187,7 @@
       <c r="Q69" s="68"/>
       <c r="R69" s="68"/>
     </row>
-    <row r="70" spans="11:18">
+    <row r="70" spans="11:18" x14ac:dyDescent="0.3">
       <c r="K70" s="68"/>
       <c r="L70" s="68"/>
       <c r="M70" s="68"/>
@@ -9197,7 +9197,7 @@
       <c r="Q70" s="68"/>
       <c r="R70" s="68"/>
     </row>
-    <row r="71" spans="11:18">
+    <row r="71" spans="11:18" x14ac:dyDescent="0.3">
       <c r="K71" s="68"/>
       <c r="L71" s="68"/>
       <c r="M71" s="68"/>
@@ -9207,7 +9207,7 @@
       <c r="Q71" s="68"/>
       <c r="R71" s="68"/>
     </row>
-    <row r="72" spans="11:18" ht="9" customHeight="1">
+    <row r="72" spans="11:18" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="K72" s="68"/>
       <c r="L72" s="68"/>
       <c r="M72" s="68"/>
@@ -9217,7 +9217,7 @@
       <c r="Q72" s="68"/>
       <c r="R72" s="68"/>
     </row>
-    <row r="73" spans="11:18">
+    <row r="73" spans="11:18" x14ac:dyDescent="0.3">
       <c r="K73" s="68"/>
       <c r="L73" s="68"/>
       <c r="M73" s="68"/>
@@ -9227,7 +9227,7 @@
       <c r="Q73" s="68"/>
       <c r="R73" s="68"/>
     </row>
-    <row r="74" spans="11:18">
+    <row r="74" spans="11:18" x14ac:dyDescent="0.3">
       <c r="K74" s="68"/>
       <c r="L74" s="68"/>
       <c r="M74" s="68"/>
@@ -9237,7 +9237,7 @@
       <c r="Q74" s="68"/>
       <c r="R74" s="68"/>
     </row>
-    <row r="75" spans="11:18">
+    <row r="75" spans="11:18" x14ac:dyDescent="0.3">
       <c r="K75" s="68"/>
       <c r="L75" s="68"/>
       <c r="M75" s="68"/>
@@ -9247,7 +9247,7 @@
       <c r="Q75" s="68"/>
       <c r="R75" s="68"/>
     </row>
-    <row r="76" spans="11:18">
+    <row r="76" spans="11:18" x14ac:dyDescent="0.3">
       <c r="K76" s="68"/>
       <c r="L76" s="68"/>
       <c r="M76" s="68"/>
@@ -9257,7 +9257,7 @@
       <c r="Q76" s="68"/>
       <c r="R76" s="68"/>
     </row>
-    <row r="77" spans="11:18">
+    <row r="77" spans="11:18" x14ac:dyDescent="0.3">
       <c r="K77" s="68"/>
       <c r="L77" s="68"/>
       <c r="M77" s="68"/>
@@ -9267,7 +9267,7 @@
       <c r="Q77" s="68"/>
       <c r="R77" s="68"/>
     </row>
-    <row r="78" spans="11:18">
+    <row r="78" spans="11:18" x14ac:dyDescent="0.3">
       <c r="K78" s="68"/>
       <c r="L78" s="68"/>
       <c r="M78" s="68"/>
@@ -9277,7 +9277,7 @@
       <c r="Q78" s="68"/>
       <c r="R78" s="68"/>
     </row>
-    <row r="79" spans="11:18">
+    <row r="79" spans="11:18" x14ac:dyDescent="0.3">
       <c r="K79" s="68"/>
       <c r="L79" s="68"/>
       <c r="M79" s="68"/>
@@ -9287,7 +9287,7 @@
       <c r="Q79" s="68"/>
       <c r="R79" s="68"/>
     </row>
-    <row r="80" spans="11:18">
+    <row r="80" spans="11:18" x14ac:dyDescent="0.3">
       <c r="K80" s="68"/>
       <c r="L80" s="68"/>
       <c r="M80" s="68"/>
@@ -9297,7 +9297,7 @@
       <c r="Q80" s="68"/>
       <c r="R80" s="68"/>
     </row>
-    <row r="81" spans="11:18">
+    <row r="81" spans="11:18" x14ac:dyDescent="0.3">
       <c r="K81" s="68"/>
       <c r="L81" s="68"/>
       <c r="M81" s="68"/>
@@ -9307,7 +9307,7 @@
       <c r="Q81" s="68"/>
       <c r="R81" s="68"/>
     </row>
-    <row r="82" spans="11:18">
+    <row r="82" spans="11:18" x14ac:dyDescent="0.3">
       <c r="K82" s="68"/>
       <c r="L82" s="68"/>
       <c r="M82" s="68"/>
@@ -9317,7 +9317,7 @@
       <c r="Q82" s="68"/>
       <c r="R82" s="68"/>
     </row>
-    <row r="83" spans="11:18">
+    <row r="83" spans="11:18" x14ac:dyDescent="0.3">
       <c r="K83" s="68"/>
       <c r="L83" s="68"/>
       <c r="M83" s="68"/>
@@ -9327,7 +9327,7 @@
       <c r="Q83" s="68"/>
       <c r="R83" s="68"/>
     </row>
-    <row r="84" spans="11:18">
+    <row r="84" spans="11:18" x14ac:dyDescent="0.3">
       <c r="K84" s="68"/>
       <c r="L84" s="68"/>
       <c r="M84" s="68"/>
@@ -9339,21 +9339,43 @@
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="L46:N46"/>
-    <mergeCell ref="E47:I47"/>
-    <mergeCell ref="L47:N47"/>
-    <mergeCell ref="L38:N38"/>
-    <mergeCell ref="E38:I38"/>
-    <mergeCell ref="E41:I41"/>
-    <mergeCell ref="L41:N41"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="L42:N42"/>
-    <mergeCell ref="L43:N43"/>
-    <mergeCell ref="E44:I44"/>
-    <mergeCell ref="L44:N44"/>
-    <mergeCell ref="E45:I45"/>
-    <mergeCell ref="E39:I39"/>
-    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="L29:N29"/>
+    <mergeCell ref="D3:J3"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="N10:N11"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="J25:N25"/>
+    <mergeCell ref="J26:N26"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="E48:I48"/>
+    <mergeCell ref="E51:I51"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="E31:I31"/>
+    <mergeCell ref="E32:I32"/>
+    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="E34:I34"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="L39:N39"/>
+    <mergeCell ref="L40:N40"/>
+    <mergeCell ref="L32:N32"/>
+    <mergeCell ref="L33:N33"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L30:N30"/>
+    <mergeCell ref="L31:N31"/>
+    <mergeCell ref="E29:I29"/>
     <mergeCell ref="J23:N23"/>
     <mergeCell ref="J24:N24"/>
     <mergeCell ref="E53:I53"/>
@@ -9370,61 +9392,39 @@
     <mergeCell ref="L52:N52"/>
     <mergeCell ref="L45:N45"/>
     <mergeCell ref="E46:I46"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L30:N30"/>
-    <mergeCell ref="L31:N31"/>
-    <mergeCell ref="E29:I29"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="L39:N39"/>
-    <mergeCell ref="L40:N40"/>
-    <mergeCell ref="L32:N32"/>
-    <mergeCell ref="L33:N33"/>
-    <mergeCell ref="L34:N34"/>
-    <mergeCell ref="E48:I48"/>
-    <mergeCell ref="E51:I51"/>
-    <mergeCell ref="E30:I30"/>
-    <mergeCell ref="E31:I31"/>
-    <mergeCell ref="E32:I32"/>
-    <mergeCell ref="E33:I33"/>
-    <mergeCell ref="E34:I34"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="L29:N29"/>
-    <mergeCell ref="D3:J3"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="N10:N11"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="J25:N25"/>
-    <mergeCell ref="J26:N26"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="L46:N46"/>
+    <mergeCell ref="E47:I47"/>
+    <mergeCell ref="L47:N47"/>
+    <mergeCell ref="L38:N38"/>
+    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="E41:I41"/>
+    <mergeCell ref="L41:N41"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="L42:N42"/>
+    <mergeCell ref="L43:N43"/>
+    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="L44:N44"/>
+    <mergeCell ref="E45:I45"/>
+    <mergeCell ref="E39:I39"/>
+    <mergeCell ref="E40:I40"/>
   </mergeCells>
   <conditionalFormatting sqref="K39">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="RECIBIDO">
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="RECIBIDO">
       <formula>NOT(ISERROR(SEARCH("RECIBIDO",K39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K39">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="PENDIENTE">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="PENDIENTE">
       <formula>NOT(ISERROR(SEARCH("PENDIENTE",K39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K40:K53">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="PENDIENTE">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="PENDIENTE">
       <formula>NOT(ISERROR(SEARCH("PENDIENTE",K40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K40:K53">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="RECIBIDO">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="RECIBIDO">
       <formula>NOT(ISERROR(SEARCH("RECIBIDO",K40)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>